<commit_message>
wrapping up Jodine budget
</commit_message>
<xml_diff>
--- a/source files/accounts_ftb04.xlsx
+++ b/source files/accounts_ftb04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT Repos/ftrack/source files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D46C45-FC83-104F-B9B3-E303DD58B3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAF9DF5-7B0E-DF41-9C49-7317DD40B4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107200" yWindow="-1100" windowWidth="38400" windowHeight="23500" xr2:uid="{339D4989-ABBB-144A-8694-33787563D3BA}"/>
+    <workbookView xWindow="-60080" yWindow="-980" windowWidth="38400" windowHeight="23500" xr2:uid="{339D4989-ABBB-144A-8694-33787563D3BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Bernice Transactional</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Vehicle Loan</t>
+  </si>
+  <si>
+    <t>Jodine Transactional</t>
+  </si>
+  <si>
+    <t>Jodine Cash</t>
+  </si>
+  <si>
+    <t>Jodine Personal Savings</t>
+  </si>
+  <si>
+    <t>Jodine Cash Savings</t>
   </si>
 </sst>
 </file>
@@ -491,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A3564C-6FD2-944E-9DE9-C9098EF02BF5}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,6 +705,50 @@
         <v>0.1484</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>